<commit_message>
Arreglo en ejemplos extra
</commit_message>
<xml_diff>
--- a/Clase Extra P2/Soluciones_Prueba.xlsx
+++ b/Clase Extra P2/Soluciones_Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minin\OneDrive\Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C99F411-24B0-44D8-BACB-623FF7440639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FAA19BA-1F39-4D67-9C76-3210BDBDC0BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15720" xr2:uid="{3ED35096-0164-405F-B810-E28154424B26}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="172">
   <si>
     <t>tiempo</t>
   </si>
@@ -1758,7 +1758,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1782,19 +1782,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2252,8 +2248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{723F5FFF-C5BC-4552-9383-66B718380C16}">
   <dimension ref="B1:I180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A164" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F173" sqref="F173"/>
+    <sheetView tabSelected="1" topLeftCell="A157" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2937,7 +2933,7 @@
         <v>68</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>72</v>
+        <v>18</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>21</v>
@@ -2945,7 +2941,7 @@
       <c r="E47" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="13" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2962,67 +2958,61 @@
       <c r="E48" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="9" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="51" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B51" s="7" t="s">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B49" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B52" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B53" s="6" t="s">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B54" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C54" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="6" t="s">
+      <c r="D54" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E53" s="6" t="s">
+      <c r="E54" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F53" s="6" t="s">
+      <c r="F54" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G53" s="6" t="s">
+      <c r="G54" s="6" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B54" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G54" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I54" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E55" s="1" t="s">
         <v>21</v>
@@ -3039,13 +3029,13 @@
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E56" s="1" t="s">
         <v>21</v>
@@ -3062,13 +3052,13 @@
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E57" s="1" t="s">
         <v>21</v>
@@ -3085,13 +3075,13 @@
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E58" s="1" t="s">
         <v>21</v>
@@ -3108,13 +3098,13 @@
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>21</v>
@@ -3131,13 +3121,13 @@
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E60" s="1" t="s">
         <v>21</v>
@@ -3154,13 +3144,13 @@
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E61" s="1" t="s">
         <v>21</v>
@@ -3177,13 +3167,13 @@
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E62" s="1" t="s">
         <v>21</v>
@@ -3200,10 +3190,10 @@
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>21</v>
@@ -3223,10 +3213,10 @@
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B64" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>85</v>
+        <v>20</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>21</v>
@@ -3241,12 +3231,12 @@
         <v>21</v>
       </c>
       <c r="I64" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B65" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>85</v>
@@ -3269,7 +3259,7 @@
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B66" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>85</v>
@@ -3292,7 +3282,7 @@
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B67" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>85</v>
@@ -3315,7 +3305,7 @@
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B68" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>85</v>
@@ -3333,18 +3323,18 @@
         <v>21</v>
       </c>
       <c r="I68" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B69" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="E69" s="1" t="s">
         <v>21</v>
@@ -3355,13 +3345,13 @@
       <c r="G69" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I69" s="4" t="s">
-        <v>88</v>
+      <c r="I69" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B70" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>21</v>
@@ -3384,7 +3374,7 @@
     </row>
     <row r="71" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B71" s="3" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>21</v>
@@ -3406,8 +3396,8 @@
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B72" s="2" t="s">
-        <v>66</v>
+      <c r="B72" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>21</v>
@@ -3430,7 +3420,7 @@
     </row>
     <row r="73" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B73" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>21</v>
@@ -3447,19 +3437,19 @@
       <c r="G73" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I73" s="5" t="s">
+      <c r="I73" s="4" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="E74" s="1" t="s">
         <v>21</v>
@@ -3470,11 +3460,13 @@
       <c r="G74" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I74" s="5"/>
+      <c r="I74" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>21</v>
@@ -3495,7 +3487,7 @@
     </row>
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B76" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>21</v>
@@ -3516,7 +3508,7 @@
     </row>
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B77" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>21</v>
@@ -3533,116 +3525,114 @@
       <c r="G77" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="I77" s="5"/>
     </row>
     <row r="78" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B78" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="79" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B79" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="80" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B80" s="7" t="s">
+      <c r="C79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B81" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="82" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B82" s="6" t="s">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B83" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C82" s="6" t="s">
+      <c r="C83" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D82" s="6" t="s">
+      <c r="D83" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E82" s="6" t="s">
+      <c r="E83" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="F82" s="6" t="s">
+      <c r="F83" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="G82" s="6" t="s">
+      <c r="G83" s="6" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="83" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B83" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I83" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B84" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>53</v>
+        <v>11</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I84" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B85" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>53</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I85" t="s">
         <v>121</v>
@@ -3650,7 +3640,7 @@
     </row>
     <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>53</v>
@@ -3659,13 +3649,13 @@
         <v>21</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I86" t="s">
         <v>121</v>
@@ -3673,7 +3663,7 @@
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B87" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>53</v>
@@ -3685,10 +3675,10 @@
         <v>21</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I87" t="s">
         <v>121</v>
@@ -3696,7 +3686,7 @@
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B88" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>53</v>
@@ -3711,21 +3701,21 @@
         <v>21</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="I88" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B89" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>12</v>
+        <v>53</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>21</v>
@@ -3737,15 +3727,15 @@
         <v>21</v>
       </c>
       <c r="I89" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B90" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>50</v>
@@ -3765,10 +3755,10 @@
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B91" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>50</v>
@@ -3788,10 +3778,10 @@
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B92" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>50</v>
@@ -3811,10 +3801,10 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" s="3" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>50</v>
@@ -3829,21 +3819,21 @@
         <v>21</v>
       </c>
       <c r="I93" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B94" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>21</v>
@@ -3852,18 +3842,18 @@
         <v>21</v>
       </c>
       <c r="I94" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B95" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E95" s="1" t="s">
         <v>22</v>
@@ -3880,13 +3870,13 @@
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E96" s="1" t="s">
         <v>22</v>
@@ -3903,13 +3893,13 @@
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E97" s="1" t="s">
         <v>22</v>
@@ -3926,13 +3916,13 @@
     </row>
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B98" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E98" s="1" t="s">
         <v>22</v>
@@ -3944,35 +3934,35 @@
         <v>21</v>
       </c>
       <c r="I98" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B99" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I99" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100" s="3" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>21</v>
@@ -3981,7 +3971,7 @@
         <v>21</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>89</v>
@@ -3994,8 +3984,8 @@
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B101" s="2" t="s">
-        <v>66</v>
+      <c r="B101" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>21</v>
@@ -4004,7 +3994,7 @@
         <v>21</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>89</v>
@@ -4018,7 +4008,7 @@
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B102" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>21</v>
@@ -4027,7 +4017,7 @@
         <v>21</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>89</v>
@@ -4041,7 +4031,7 @@
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B103" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>21</v>
@@ -4050,7 +4040,7 @@
         <v>21</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>89</v>
@@ -4059,12 +4049,12 @@
         <v>21</v>
       </c>
       <c r="I103" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B104" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>21</v>
@@ -4073,21 +4063,21 @@
         <v>21</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>15</v>
+        <v>89</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>61</v>
+        <v>21</v>
       </c>
       <c r="I104" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B105" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>21</v>
@@ -4099,7 +4089,7 @@
         <v>21</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>61</v>
@@ -4110,7 +4100,7 @@
     </row>
     <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B106" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>21</v>
@@ -4122,7 +4112,7 @@
         <v>21</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>61</v>
@@ -4133,7 +4123,7 @@
     </row>
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B107" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>21</v>
@@ -4145,7 +4135,7 @@
         <v>21</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>61</v>
@@ -4156,7 +4146,7 @@
     </row>
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B108" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>21</v>
@@ -4168,21 +4158,21 @@
         <v>21</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>61</v>
       </c>
       <c r="I108" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B109" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>21</v>
@@ -4191,18 +4181,18 @@
         <v>21</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="I109" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B110" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>69</v>
@@ -4217,7 +4207,7 @@
         <v>21</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I110" t="s">
         <v>131</v>
@@ -4225,7 +4215,7 @@
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B111" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>69</v>
@@ -4240,7 +4230,7 @@
         <v>21</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I111" t="s">
         <v>131</v>
@@ -4248,7 +4238,7 @@
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B112" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>69</v>
@@ -4263,7 +4253,7 @@
         <v>21</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I112" t="s">
         <v>131</v>
@@ -4271,7 +4261,7 @@
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B113" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>69</v>
@@ -4286,21 +4276,21 @@
         <v>21</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I113" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B114" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="E114" s="1" t="s">
         <v>21</v>
@@ -4309,15 +4299,15 @@
         <v>21</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I114" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B115" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>21</v>
@@ -4340,7 +4330,7 @@
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B116" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C116" s="1" t="s">
         <v>21</v>
@@ -4363,7 +4353,7 @@
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B117" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C117" s="1" t="s">
         <v>21</v>
@@ -4386,7 +4376,7 @@
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B118" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C118" s="1" t="s">
         <v>21</v>
@@ -4404,21 +4394,21 @@
         <v>21</v>
       </c>
       <c r="I118" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B119" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C119" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="F119" s="1" t="s">
         <v>21</v>
@@ -4427,12 +4417,12 @@
         <v>21</v>
       </c>
       <c r="I119" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B120" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C120" s="1" t="s">
         <v>21</v>
@@ -4455,7 +4445,7 @@
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B121" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C121" s="1" t="s">
         <v>21</v>
@@ -4478,7 +4468,7 @@
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B122" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>21</v>
@@ -4501,7 +4491,7 @@
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B123" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C123" s="1" t="s">
         <v>21</v>
@@ -4519,12 +4509,12 @@
         <v>21</v>
       </c>
       <c r="I123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B124" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C124" s="1" t="s">
         <v>21</v>
@@ -4533,21 +4523,21 @@
         <v>21</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I124" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B125" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C125" s="1" t="s">
         <v>21</v>
@@ -4570,7 +4560,7 @@
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B126" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C126" s="1" t="s">
         <v>21</v>
@@ -4593,7 +4583,7 @@
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B127" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C127" s="1" t="s">
         <v>21</v>
@@ -4616,7 +4606,7 @@
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B128" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C128" s="1" t="s">
         <v>21</v>
@@ -4634,12 +4624,12 @@
         <v>21</v>
       </c>
       <c r="I128" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B129" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C129" s="1" t="s">
         <v>21</v>
@@ -4651,18 +4641,18 @@
         <v>21</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I129" s="4" t="s">
-        <v>139</v>
+        <v>21</v>
+      </c>
+      <c r="I129" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B130" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C130" s="1" t="s">
         <v>21</v>
@@ -4685,7 +4675,7 @@
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B131" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C131" s="1" t="s">
         <v>21</v>
@@ -4708,7 +4698,7 @@
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B132" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C132" s="1" t="s">
         <v>21</v>
@@ -4731,7 +4721,7 @@
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B133" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C133" s="1" t="s">
         <v>21</v>
@@ -4752,314 +4742,312 @@
         <v>139</v>
       </c>
     </row>
-    <row r="136" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B136" s="7" t="s">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B134" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F134" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I134" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="137" spans="2:9" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B137" s="7" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="138" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B138" s="6" t="s">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B139" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C138" s="6" t="s">
+      <c r="C139" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D138" s="6" t="s">
+      <c r="D139" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="E138" s="12" t="s">
+      <c r="E139" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="F138" s="12"/>
-      <c r="G138" s="12"/>
-    </row>
-    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B139" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C139" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D139" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="E139" s="13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F139" s="13"/>
-      <c r="G139" s="13"/>
+      <c r="F139" s="11"/>
+      <c r="G139" s="11"/>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B140" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E140" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E140" t="s">
         <v>141</v>
       </c>
-      <c r="F140" s="13"/>
-      <c r="G140" s="13"/>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B141" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C141" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="E141" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E141" t="s">
         <v>141</v>
       </c>
-      <c r="F141" s="13"/>
-      <c r="G141" s="13"/>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B142" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C142" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D142" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E142" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B143" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C142" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D142" s="1" t="s">
+      <c r="C143" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D143" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E142" s="13" t="s">
+      <c r="E143" t="s">
         <v>146</v>
       </c>
-      <c r="F142" s="13"/>
-      <c r="G142" s="13" t="s">
+      <c r="G143" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="143" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B143" s="14" t="s">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B144" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C143" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D143" s="15" t="s">
+      <c r="C144" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D144" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E143" s="13" t="s">
+      <c r="E144" t="s">
         <v>146</v>
       </c>
-      <c r="F143" s="11"/>
-      <c r="G143" t="s">
+      <c r="G144" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B144" s="14" t="s">
+    <row r="145" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B145" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C144" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D144" s="15" t="s">
+      <c r="C145" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D145" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E144" s="13" t="s">
+      <c r="E145" t="s">
         <v>150</v>
       </c>
-      <c r="F144" s="11"/>
-    </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B145" s="14" t="s">
+    </row>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B146" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C145" s="15" t="s">
+      <c r="C146" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D145" s="15" t="s">
+      <c r="D146" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E145" s="13" t="s">
+      <c r="E146" t="s">
         <v>152</v>
       </c>
-      <c r="F145" s="11"/>
-    </row>
-    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B146" s="14" t="s">
+    </row>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B147" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C146" s="15" t="s">
+      <c r="C147" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D146" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E146" s="13" t="s">
+      <c r="D147" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E147" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="147" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B147" s="14" t="s">
+    <row r="148" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B148" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C147" s="15" t="s">
+      <c r="C148" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D147" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E147" s="13" t="s">
+      <c r="D148" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E148" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B148" s="14" t="s">
+    <row r="149" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B149" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C148" s="15" t="s">
+      <c r="C149" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D148" s="15" t="s">
+      <c r="D149" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E148" s="13" t="s">
+      <c r="E149" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="149" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B149" s="14" t="s">
+    <row r="150" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B150" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C149" s="15" t="s">
+      <c r="C150" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D149" s="15" t="s">
+      <c r="D150" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E149" s="13" t="s">
+      <c r="E150" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="150" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B150" s="14" t="s">
+    <row r="151" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B151" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C150" s="15" t="s">
+      <c r="C151" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D150" s="15" t="s">
+      <c r="D151" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E150" s="13" t="s">
+      <c r="E151" t="s">
         <v>156</v>
       </c>
-      <c r="F150" s="11"/>
-    </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B151" s="14" t="s">
+    </row>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B152" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C151" s="15" t="s">
+      <c r="C152" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D151" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E151" s="13" t="s">
+      <c r="D152" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E152" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B152" s="14" t="s">
+    <row r="153" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B153" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C152" s="15" t="s">
+      <c r="C153" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D152" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E152" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B153" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C153" s="15" t="s">
-        <v>158</v>
-      </c>
-      <c r="D153" s="15" t="s">
+      <c r="D153" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E153" s="4" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B154" s="14" t="s">
+    <row r="154" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B154" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C154" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D154" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E154" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B155" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C154" s="15" t="s">
+      <c r="C155" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D154" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E154" s="5" t="s">
+      <c r="D155" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E155" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="155" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B155" s="16" t="s">
+    <row r="156" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B156" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="C155" s="16"/>
-      <c r="D155" s="16"/>
-    </row>
-    <row r="158" spans="2:6" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="B158" s="7" t="s">
+      <c r="C156" s="12"/>
+      <c r="D156" s="12"/>
+    </row>
+    <row r="159" spans="2:5" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="B159" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B160" s="6" t="s">
+    <row r="161" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B161" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C160" s="6" t="s">
+      <c r="C161" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D160" s="6" t="s">
+      <c r="D161" s="6" t="s">
         <v>79</v>
-      </c>
-    </row>
-    <row r="161" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B161" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C161" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E161" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="162" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B162" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E162" t="s">
         <v>161</v>
@@ -5067,13 +5055,13 @@
     </row>
     <row r="163" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B163" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E163" t="s">
         <v>161</v>
@@ -5081,23 +5069,23 @@
     </row>
     <row r="164" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B164" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C164" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D164" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E164" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B165" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C164" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D164" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E164" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="165" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B165" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C165" s="15" t="s">
+      <c r="C165" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D165" s="1" t="s">
@@ -5108,69 +5096,69 @@
       </c>
     </row>
     <row r="166" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B166" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C166" s="15" t="s">
+      <c r="B166" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C166" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D166" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E166" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B167" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C167" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D167" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E167" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="167" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B167" s="14" t="s">
+    <row r="168" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B168" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C167" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D167" s="15" t="s">
+      <c r="C168" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D168" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E167" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="168" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B168" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C168" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D168" s="15" t="s">
-        <v>11</v>
       </c>
       <c r="E168" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="169" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B169" s="14" t="s">
+      <c r="B169" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C169" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D169" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E169" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B170" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C169" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D169" s="15" t="s">
-        <v>151</v>
-      </c>
-      <c r="E169" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="170" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B170" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C170" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D170" s="15" t="s">
+      <c r="C170" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D170" s="1" t="s">
         <v>151</v>
       </c>
       <c r="E170" t="s">
@@ -5178,41 +5166,41 @@
       </c>
     </row>
     <row r="171" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B171" s="14" t="s">
+      <c r="B171" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E171" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B172" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C171" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D171" s="15" t="s">
+      <c r="C172" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D172" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E171" t="s">
+      <c r="E172" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="172" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B172" s="14" t="s">
+    <row r="173" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B173" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C172" s="15" t="s">
+      <c r="C173" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D172" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E172" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="173" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B173" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C173" s="15" t="s">
-        <v>163</v>
-      </c>
-      <c r="D173" s="15" t="s">
+      <c r="D173" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E173" t="s">
@@ -5220,128 +5208,137 @@
       </c>
     </row>
     <row r="174" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B174" s="14" t="s">
+      <c r="B174" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E174" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B175" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C174" s="15" t="s">
+      <c r="C175" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="D174" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E174" t="s">
+      <c r="D175" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E175" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="175" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B175" s="14" t="s">
+    <row r="176" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B176" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C175" s="15" t="s">
+      <c r="C176" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D175" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E175" t="s">
+      <c r="D176" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E176" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="176" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B176" s="14" t="s">
+    <row r="177" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B177" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C176" s="15" t="s">
+      <c r="C177" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D176" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E176" s="4" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B177" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C177" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D177" s="15" t="s">
+      <c r="D177" s="1" t="s">
         <v>21</v>
       </c>
       <c r="E177" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B178" s="14" t="s">
+    <row r="178" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B178" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E178" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B179" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C178" s="15" t="s">
+      <c r="C179" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D178" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E178" s="17" t="s">
+      <c r="D179" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E179" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="F178" s="11"/>
-    </row>
-    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B179" s="16" t="s">
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B180" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="C179" s="16"/>
-      <c r="D179" s="16"/>
-      <c r="E179" s="17"/>
-      <c r="F179" s="11"/>
-    </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="F180" s="11"/>
+      <c r="C180" s="12"/>
+      <c r="D180" s="12"/>
+      <c r="E180" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B155:D155"/>
-    <mergeCell ref="B179:D179"/>
+    <mergeCell ref="B156:D156"/>
+    <mergeCell ref="B180:D180"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="C114:C133">
+  <conditionalFormatting sqref="C115:C134">
     <cfRule type="uniqueValues" dxfId="11" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D109:D113">
+  <conditionalFormatting sqref="D110:D114">
     <cfRule type="uniqueValues" dxfId="10" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D119:D123">
+  <conditionalFormatting sqref="D120:D124">
     <cfRule type="uniqueValues" dxfId="9" priority="7"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D124:D128">
+  <conditionalFormatting sqref="D125:D129">
     <cfRule type="uniqueValues" dxfId="8" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D129:D133">
+  <conditionalFormatting sqref="D130:D134">
     <cfRule type="uniqueValues" dxfId="7" priority="5"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E109:E118">
+  <conditionalFormatting sqref="E110:E119">
     <cfRule type="uniqueValues" dxfId="6" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E124:E128">
+  <conditionalFormatting sqref="E125:E129">
     <cfRule type="uniqueValues" dxfId="5" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E129:E133">
+  <conditionalFormatting sqref="E130:E134">
     <cfRule type="uniqueValues" dxfId="4" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F109:F123">
+  <conditionalFormatting sqref="F110:F124">
     <cfRule type="uniqueValues" dxfId="3" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F129:F133">
+  <conditionalFormatting sqref="F130:F134">
     <cfRule type="uniqueValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G114:G118">
+  <conditionalFormatting sqref="G115:G119">
     <cfRule type="uniqueValues" dxfId="1" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G119:G128">
+  <conditionalFormatting sqref="G120:G129">
     <cfRule type="uniqueValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>